<commit_message>
first commit for api
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TD\Desktop\full stack training\web0\session nine\myPractice\API\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B98F64D-6FFC-49C3-AAEE-B023EE0C3D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82BCD95F-B1D7-4107-B820-3A49D4A49A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -392,7 +392,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>